<commit_message>
Fourth Commit by Somnath Baul
</commit_message>
<xml_diff>
--- a/Excel_Format_As_Table.xlsx
+++ b/Excel_Format_As_Table.xlsx
@@ -31,13 +31,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <i val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,8 +67,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -91,7 +99,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1">
+    <row r="1" s="1" customFormat="true">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>